<commit_message>
ajout lecture tension batteries 1s / 2s
</commit_message>
<xml_diff>
--- a/Kicad/STM32F412ZGT6_GPIO_Interfaces.xlsx
+++ b/Kicad/STM32F412ZGT6_GPIO_Interfaces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gagno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gagno\OneDrive\Documents\Github\Ordinateur-de-bord\Kicad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1255BA-302E-4702-AC22-4B83C56D6E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C2D46D-2E42-4B3F-A39A-19B8AB03A68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2625" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -904,28 +904,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -937,73 +997,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1361,7 +1355,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:N89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
@@ -1414,16 +1408,16 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="52">
         <v>1</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="47" t="s">
         <v>70</v>
       </c>
       <c r="F3" s="15" t="s">
@@ -1438,7 +1432,7 @@
       <c r="I3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="50" t="s">
         <v>94</v>
       </c>
       <c r="L3" s="22" t="s">
@@ -1446,10 +1440,10 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
       <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1462,16 +1456,16 @@
       <c r="I4" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K4" s="26"/>
+      <c r="K4" s="50"/>
       <c r="L4" s="23" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1492,10 +1486,10 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
       <c r="F6" s="2" t="s">
         <v>64</v>
       </c>
@@ -1508,7 +1502,7 @@
       <c r="I6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="50" t="s">
         <v>101</v>
       </c>
       <c r="L6" s="22" t="s">
@@ -1516,14 +1510,14 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
-      <c r="C7" s="27">
+      <c r="B7" s="50"/>
+      <c r="C7" s="52">
         <v>2</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="47" t="s">
         <v>71</v>
       </c>
       <c r="F7" s="15" t="s">
@@ -1538,16 +1532,16 @@
       <c r="I7" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K7" s="26"/>
+      <c r="K7" s="50"/>
       <c r="L7" s="23" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1568,10 +1562,10 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1592,10 +1586,10 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="9" t="s">
         <v>64</v>
       </c>
@@ -1608,19 +1602,19 @@
       <c r="I10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="41" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="27">
+      <c r="B11" s="50"/>
+      <c r="C11" s="52">
         <v>3</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="47" t="s">
         <v>71</v>
       </c>
       <c r="F11" s="15" t="s">
@@ -1635,13 +1629,13 @@
       <c r="I11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="37"/>
+      <c r="K11" s="42"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
@@ -1654,13 +1648,13 @@
       <c r="I12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="42"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1673,13 +1667,13 @@
       <c r="I13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="42"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
       <c r="F14" s="9" t="s">
         <v>64</v>
       </c>
@@ -1692,17 +1686,17 @@
       <c r="I14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K14" s="37"/>
+      <c r="K14" s="42"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="27">
+      <c r="B15" s="50"/>
+      <c r="C15" s="52">
         <v>4</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="47" t="s">
         <v>70</v>
       </c>
       <c r="F15" s="15" t="s">
@@ -1717,13 +1711,13 @@
       <c r="I15" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="K15" s="37"/>
+      <c r="K15" s="42"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
@@ -1736,13 +1730,13 @@
       <c r="I16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K16" s="37"/>
+      <c r="K16" s="42"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1755,13 +1749,13 @@
       <c r="I17" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="37"/>
+      <c r="K17" s="42"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
       <c r="F18" s="9" t="s">
         <v>64</v>
       </c>
@@ -1774,17 +1768,17 @@
       <c r="I18" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="37"/>
+      <c r="K18" s="42"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
-      <c r="C19" s="27">
+      <c r="B19" s="50"/>
+      <c r="C19" s="52">
         <v>5</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="47" t="s">
         <v>70</v>
       </c>
       <c r="F19" s="15" t="s">
@@ -1799,13 +1793,13 @@
       <c r="I19" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="37"/>
+      <c r="K19" s="42"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="2" t="s">
         <v>2</v>
       </c>
@@ -1818,13 +1812,13 @@
       <c r="I20" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="42"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1837,13 +1831,13 @@
       <c r="I21" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="37"/>
+      <c r="K21" s="42"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
       <c r="F22" s="9" t="s">
         <v>64</v>
       </c>
@@ -1856,19 +1850,19 @@
       <c r="I22" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="37"/>
+      <c r="K22" s="42"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="52">
         <v>1</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="47" t="s">
         <v>68</v>
       </c>
       <c r="F23" s="15" t="s">
@@ -1883,13 +1877,13 @@
       <c r="I23" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K23" s="37"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
-      <c r="C24" s="28"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="2" t="s">
         <v>5</v>
       </c>
@@ -1902,13 +1896,13 @@
       <c r="I24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K24" s="37"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="26"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1921,13 +1915,13 @@
       <c r="I25" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K25" s="37"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1940,13 +1934,13 @@
       <c r="I26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K26" s="38"/>
+      <c r="K26" s="44"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="26"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1964,14 +1958,14 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
-      <c r="C28" s="27">
+      <c r="B28" s="50"/>
+      <c r="C28" s="52">
         <v>2</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="47" t="s">
         <v>69</v>
       </c>
       <c r="F28" s="15" t="s">
@@ -1988,10 +1982,10 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="2" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2000,10 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
       <c r="F30" s="2" t="s">
         <v>6</v>
       </c>
@@ -2024,10 +2018,10 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="26"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="2" t="s">
         <v>7</v>
       </c>
@@ -2042,10 +2036,10 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="26"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="9" t="s">
         <v>8</v>
       </c>
@@ -2060,14 +2054,14 @@
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="26"/>
-      <c r="C33" s="27">
+      <c r="B33" s="50"/>
+      <c r="C33" s="52">
         <v>3</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E33" s="47" t="s">
         <v>69</v>
       </c>
       <c r="F33" s="15" t="s">
@@ -2082,20 +2076,20 @@
       <c r="I33" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="25" t="s">
+      <c r="K33" s="56" t="s">
         <v>112</v>
       </c>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
       <c r="N33" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="26"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
       <c r="F34" s="2" t="s">
         <v>5</v>
       </c>
@@ -2123,10 +2117,10 @@
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="2" t="s">
         <v>6</v>
       </c>
@@ -2150,10 +2144,10 @@
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
       <c r="F36" s="2" t="s">
         <v>7</v>
       </c>
@@ -2181,10 +2175,10 @@
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B37" s="26"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="9" t="s">
         <v>8</v>
       </c>
@@ -2212,14 +2206,14 @@
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B38" s="26"/>
-      <c r="C38" s="27">
+      <c r="B38" s="50"/>
+      <c r="C38" s="52">
         <v>6</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="47" t="s">
         <v>68</v>
       </c>
       <c r="F38" s="15" t="s">
@@ -2245,10 +2239,10 @@
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B39" s="26"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2276,10 +2270,10 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B40" s="26"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
       <c r="F40" s="2" t="s">
         <v>6</v>
       </c>
@@ -2303,10 +2297,10 @@
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="26"/>
-      <c r="C41" s="28"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="2" t="s">
         <v>7</v>
       </c>
@@ -2321,10 +2315,10 @@
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B42" s="26"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
       <c r="F42" s="9" t="s">
         <v>8</v>
       </c>
@@ -2339,16 +2333,16 @@
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="27">
+      <c r="C43" s="52">
         <v>1</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="53" t="s">
         <v>92</v>
       </c>
       <c r="F43" s="15" t="s">
@@ -2365,10 +2359,10 @@
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B44" s="26"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="34"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="54"/>
       <c r="F44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2383,10 +2377,10 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B45" s="26"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="35"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="55"/>
       <c r="F45" s="9" t="s">
         <v>11</v>
       </c>
@@ -2401,14 +2395,14 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B46" s="26"/>
-      <c r="C46" s="27">
+      <c r="B46" s="50"/>
+      <c r="C46" s="52">
         <v>2</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="E46" s="47" t="s">
         <v>67</v>
       </c>
       <c r="F46" s="15" t="s">
@@ -2425,10 +2419,10 @@
       </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
-      <c r="C47" s="28"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="2" t="s">
         <v>10</v>
       </c>
@@ -2443,10 +2437,10 @@
       </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B48" s="26"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
       <c r="F48" s="9" t="s">
         <v>11</v>
       </c>
@@ -2461,14 +2455,14 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="26"/>
-      <c r="C49" s="28">
+      <c r="B49" s="50"/>
+      <c r="C49" s="43">
         <v>3</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="31" t="s">
+      <c r="E49" s="48" t="s">
         <v>67</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -2485,10 +2479,10 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="26"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
       <c r="F50" s="2" t="s">
         <v>10</v>
       </c>
@@ -2503,10 +2497,10 @@
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="26"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="51"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
       <c r="F51" s="9" t="s">
         <v>11</v>
       </c>
@@ -2521,7 +2515,7 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="50" t="s">
         <v>83</v>
       </c>
       <c r="C52" s="18">
@@ -2549,7 +2543,7 @@
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="26"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="19">
         <v>1</v>
       </c>
@@ -2575,7 +2569,7 @@
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="26"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="19">
         <v>2</v>
       </c>
@@ -2601,7 +2595,7 @@
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="26"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="19">
         <v>3</v>
       </c>
@@ -2627,7 +2621,7 @@
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="26"/>
+      <c r="B56" s="50"/>
       <c r="C56" s="19">
         <v>4</v>
       </c>
@@ -2653,7 +2647,7 @@
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="26"/>
+      <c r="B57" s="50"/>
       <c r="C57" s="19">
         <v>5</v>
       </c>
@@ -2679,7 +2673,7 @@
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="26"/>
+      <c r="B58" s="50"/>
       <c r="C58" s="19">
         <v>6</v>
       </c>
@@ -2705,7 +2699,7 @@
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="26"/>
+      <c r="B59" s="50"/>
       <c r="C59" s="19">
         <v>7</v>
       </c>
@@ -2731,7 +2725,7 @@
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="26"/>
+      <c r="B60" s="50"/>
       <c r="C60" s="19">
         <v>8</v>
       </c>
@@ -2757,7 +2751,7 @@
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="26"/>
+      <c r="B61" s="50"/>
       <c r="C61" s="19">
         <v>9</v>
       </c>
@@ -2783,7 +2777,7 @@
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="26"/>
+      <c r="B62" s="50"/>
       <c r="C62" s="19">
         <v>10</v>
       </c>
@@ -2809,7 +2803,7 @@
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="26"/>
+      <c r="B63" s="50"/>
       <c r="C63" s="19">
         <v>11</v>
       </c>
@@ -2838,7 +2832,7 @@
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="26"/>
+      <c r="B64" s="50"/>
       <c r="C64" s="19">
         <v>12</v>
       </c>
@@ -2867,7 +2861,7 @@
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" s="26"/>
+      <c r="B65" s="50"/>
       <c r="C65" s="19">
         <v>13</v>
       </c>
@@ -2893,7 +2887,7 @@
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="26"/>
+      <c r="B66" s="50"/>
       <c r="C66" s="19">
         <v>14</v>
       </c>
@@ -2919,7 +2913,7 @@
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="26"/>
+      <c r="B67" s="50"/>
       <c r="C67" s="20">
         <v>15</v>
       </c>
@@ -2949,7 +2943,7 @@
       <c r="K67" s="46"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="41" t="s">
         <v>94</v>
       </c>
       <c r="C68" s="14" t="s">
@@ -2978,28 +2972,28 @@
       <c r="J68" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="K68" s="42"/>
+      <c r="K68" s="26"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" s="37"/>
+      <c r="B69" s="42"/>
       <c r="C69" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D69" s="39" t="str">
+      <c r="D69" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E69" s="39" t="str">
+      <c r="E69" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F69" s="39" t="s">
+      <c r="F69" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G69" s="39" t="s">
+      <c r="G69" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H69" s="39" t="s">
+      <c r="H69" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I69" s="7" t="s">
@@ -3008,28 +3002,28 @@
       <c r="J69" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="K69" s="42"/>
+      <c r="K69" s="26"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" s="37"/>
+      <c r="B70" s="42"/>
       <c r="C70" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D70" s="39" t="str">
+      <c r="D70" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E70" s="39" t="str">
+      <c r="E70" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F70" s="39" t="s">
+      <c r="F70" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G70" s="39" t="s">
+      <c r="G70" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="H70" s="39" t="s">
+      <c r="H70" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I70" s="7" t="s">
@@ -3038,28 +3032,28 @@
       <c r="J70" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="K70" s="42"/>
+      <c r="K70" s="26"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="37"/>
+      <c r="B71" s="42"/>
       <c r="C71" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D71" s="39" t="str">
+      <c r="D71" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E71" s="39" t="str">
+      <c r="E71" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F71" s="39" t="s">
+      <c r="F71" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G71" s="39" t="s">
+      <c r="G71" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H71" s="39" t="s">
+      <c r="H71" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I71" s="7" t="s">
@@ -3068,28 +3062,28 @@
       <c r="J71" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="K71" s="42"/>
+      <c r="K71" s="26"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B72" s="37"/>
+      <c r="B72" s="42"/>
       <c r="C72" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D72" s="39" t="str">
+      <c r="D72" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E72" s="39" t="str">
+      <c r="E72" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F72" s="39" t="s">
+      <c r="F72" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G72" s="39" t="s">
+      <c r="G72" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H72" s="39" t="s">
+      <c r="H72" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I72" s="7" t="s">
@@ -3098,28 +3092,28 @@
       <c r="J72" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="K72" s="42"/>
+      <c r="K72" s="26"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="37"/>
+      <c r="B73" s="42"/>
       <c r="C73" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="D73" s="39" t="str">
+      <c r="D73" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E73" s="39" t="str">
+      <c r="E73" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F73" s="39" t="s">
+      <c r="F73" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G73" s="39" t="s">
+      <c r="G73" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H73" s="39" t="s">
+      <c r="H73" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I73" s="7" t="s">
@@ -3128,28 +3122,28 @@
       <c r="J73" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="K73" s="42"/>
+      <c r="K73" s="26"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="37"/>
+      <c r="B74" s="42"/>
       <c r="C74" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="39" t="str">
+      <c r="D74" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E74" s="39" t="str">
+      <c r="E74" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F74" s="39" t="s">
+      <c r="F74" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G74" s="39" t="s">
+      <c r="G74" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H74" s="39" t="s">
+      <c r="H74" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I74" s="7" t="s">
@@ -3158,28 +3152,28 @@
       <c r="J74" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K74" s="42"/>
+      <c r="K74" s="26"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="37"/>
+      <c r="B75" s="42"/>
       <c r="C75" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D75" s="39" t="str">
+      <c r="D75" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E75" s="39" t="str">
+      <c r="E75" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F75" s="39" t="s">
+      <c r="F75" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G75" s="39" t="s">
+      <c r="G75" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H75" s="39" t="s">
+      <c r="H75" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I75" s="7" t="s">
@@ -3188,28 +3182,28 @@
       <c r="J75" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="K75" s="42"/>
+      <c r="K75" s="26"/>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" s="37"/>
-      <c r="C76" s="47" t="s">
+      <c r="B76" s="42"/>
+      <c r="C76" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D76" s="39" t="str">
+      <c r="D76" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E76" s="39" t="str">
+      <c r="E76" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F76" s="39" t="s">
+      <c r="F76" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="G76" s="39" t="s">
+      <c r="G76" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H76" s="39" t="s">
+      <c r="H76" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I76" s="7" t="s">
@@ -3218,30 +3212,30 @@
       <c r="J76" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="K76" s="43" t="s">
+      <c r="K76" s="27" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" s="37"/>
-      <c r="C77" s="47" t="s">
+      <c r="B77" s="42"/>
+      <c r="C77" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="D77" s="39" t="str">
+      <c r="D77" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E77" s="39" t="str">
+      <c r="E77" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F77" s="40" t="s">
+      <c r="F77" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G77" s="39" t="s">
+      <c r="G77" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H77" s="39" t="s">
+      <c r="H77" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I77" s="7" t="s">
@@ -3250,30 +3244,30 @@
       <c r="J77" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="K77" s="43" t="s">
+      <c r="K77" s="27" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" s="37"/>
+      <c r="B78" s="42"/>
       <c r="C78" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D78" s="39" t="str">
+      <c r="D78" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E78" s="39" t="str">
+      <c r="E78" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F78" s="40" t="s">
+      <c r="F78" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="G78" s="39" t="s">
+      <c r="G78" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H78" s="39" t="s">
+      <c r="H78" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I78" s="7" t="s">
@@ -3282,94 +3276,94 @@
       <c r="J78" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="K78" s="42" t="s">
+      <c r="K78" s="26" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" s="37"/>
+      <c r="B79" s="42"/>
       <c r="C79" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="D79" s="39" t="str">
+      <c r="D79" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E79" s="39" t="str">
+      <c r="E79" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F79" s="40" t="s">
+      <c r="F79" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="G79" s="39" t="s">
+      <c r="G79" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H79" s="39" t="s">
+      <c r="H79" s="2" t="s">
         <v>87</v>
       </c>
       <c r="I79" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="J79" s="44" t="s">
+      <c r="J79" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="K79" s="42" t="s">
+      <c r="K79" s="26" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" s="37"/>
-      <c r="C80" s="47" t="s">
+      <c r="B80" s="42"/>
+      <c r="C80" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="D80" s="48" t="str">
+      <c r="D80" s="30" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E80" s="48" t="str">
+      <c r="E80" s="30" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F80" s="49" t="s">
+      <c r="F80" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="G80" s="48" t="s">
+      <c r="G80" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H80" s="48" t="s">
-        <v>87</v>
-      </c>
-      <c r="I80" s="50" t="s">
+      <c r="H80" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="I80" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="J80" s="47" t="s">
+      <c r="J80" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="K80" s="51" t="s">
+      <c r="K80" s="33" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="81" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B81" s="37"/>
+      <c r="B81" s="42"/>
       <c r="C81" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="D81" s="39" t="str">
+      <c r="D81" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="E81" s="39" t="str">
+      <c r="E81" s="2" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
       </c>
-      <c r="F81" s="41" t="s">
+      <c r="F81" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G81" s="39" t="s">
+      <c r="G81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H81" s="39" t="s">
+      <c r="H81" s="2" t="s">
         <v>171</v>
       </c>
       <c r="I81" s="7" t="str">
@@ -3379,24 +3373,24 @@
       <c r="J81" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="K81" s="43" t="s">
+      <c r="K81" s="27" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="82" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B82" s="37"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="53"/>
-      <c r="E82" s="53"/>
-      <c r="F82" s="53"/>
-      <c r="G82" s="53"/>
-      <c r="H82" s="53"/>
-      <c r="I82" s="54"/>
-      <c r="J82" s="52"/>
-      <c r="K82" s="54"/>
+      <c r="B82" s="42"/>
+      <c r="C82" s="34"/>
+      <c r="D82" s="35"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="35"/>
+      <c r="G82" s="35"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="36"/>
+      <c r="J82" s="34"/>
+      <c r="K82" s="36"/>
     </row>
     <row r="83" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B83" s="37"/>
+      <c r="B83" s="42"/>
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="15"/>
@@ -3406,38 +3400,38 @@
       <c r="K83" s="7"/>
     </row>
     <row r="84" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B84" s="28"/>
-      <c r="C84" s="47" t="s">
+      <c r="B84" s="43"/>
+      <c r="C84" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="D84" s="48"/>
-      <c r="E84" s="48"/>
-      <c r="F84" s="48"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="48"/>
-      <c r="I84" s="50"/>
-      <c r="J84" s="55" t="s">
+      <c r="D84" s="30"/>
+      <c r="E84" s="30"/>
+      <c r="F84" s="30"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="32"/>
+      <c r="J84" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="K84" s="51" t="s">
+      <c r="K84" s="33" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="85" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B85" s="37"/>
-      <c r="C85" s="47" t="s">
+      <c r="B85" s="42"/>
+      <c r="C85" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="D85" s="48"/>
-      <c r="E85" s="48"/>
-      <c r="F85" s="48"/>
-      <c r="G85" s="48"/>
-      <c r="H85" s="48"/>
-      <c r="I85" s="50"/>
-      <c r="J85" s="47" t="s">
+      <c r="D85" s="30"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="30"/>
+      <c r="G85" s="30"/>
+      <c r="H85" s="30"/>
+      <c r="I85" s="32"/>
+      <c r="J85" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="K85" s="51" t="s">
+      <c r="K85" s="33" t="s">
         <v>184</v>
       </c>
       <c r="L85" s="1" t="s">
@@ -3445,18 +3439,18 @@
       </c>
     </row>
     <row r="86" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B86" s="38"/>
-      <c r="C86" s="56" t="s">
+      <c r="B86" s="44"/>
+      <c r="C86" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="D86" s="57"/>
-      <c r="E86" s="57"/>
-      <c r="F86" s="57"/>
-      <c r="G86" s="57"/>
-      <c r="H86" s="57"/>
-      <c r="I86" s="58"/>
-      <c r="J86" s="56"/>
-      <c r="K86" s="58"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="39"/>
+      <c r="G86" s="39"/>
+      <c r="H86" s="39"/>
+      <c r="I86" s="40"/>
+      <c r="J86" s="38"/>
+      <c r="K86" s="40"/>
       <c r="L86" s="1" t="s">
         <v>188</v>
       </c>
@@ -3472,12 +3466,20 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B68:B86"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="E11:E14"/>
-    <mergeCell ref="E15:E18"/>
-    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K10:K26"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="C19:C22"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="D7:D10"/>
@@ -3488,13 +3490,19 @@
     <mergeCell ref="C49:C51"/>
     <mergeCell ref="B43:B51"/>
     <mergeCell ref="D43:D45"/>
-    <mergeCell ref="E49:E51"/>
     <mergeCell ref="C23:C27"/>
     <mergeCell ref="C28:C32"/>
     <mergeCell ref="C33:C37"/>
     <mergeCell ref="C38:C42"/>
     <mergeCell ref="D38:D42"/>
     <mergeCell ref="D28:D32"/>
+    <mergeCell ref="B68:B86"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="E19:E22"/>
+    <mergeCell ref="E49:E51"/>
     <mergeCell ref="D33:D37"/>
     <mergeCell ref="E23:E27"/>
     <mergeCell ref="E28:E32"/>
@@ -3504,20 +3512,6 @@
     <mergeCell ref="D23:D27"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="B23:B42"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="B3:B22"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K10:K26"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="E3:E6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>